<commit_message>
Исправлен fatal bug в TranzistorsTNVEDCode
</commit_message>
<xml_diff>
--- a/TranzistorsTNVEDCode/tranzistorsCode.xlsx
+++ b/TranzistorsTNVEDCode/tranzistorsCode.xlsx
@@ -341,16 +341,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D700"/>
+  <dimension ref="A1:D701"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A691" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A691" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2503,6 +2504,9 @@
     <row r="700" spans="1:1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A700" s="2"/>
     </row>
+    <row r="701" spans="1:1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A701" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>